<commit_message>
Added resources S_009_MAP-Fällung and S_010_Strippung und saure Wäsche
Added ORDER BY to SQL query so that resource names fetched are ordered by ressource, kategorieIndex
</commit_message>
<xml_diff>
--- a/Massnahmenliste.xlsx
+++ b/Massnahmenliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fl-al\Google Drive\R\R2Q_App\R2Q_App\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pramit\Documents\work\R2Q-Shiny-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1238D281-8D9C-40FE-9862-AC081F6746E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3782B5DC-BBAE-44FC-82FE-B33BF1B5DF26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35190" yWindow="2790" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
   <si>
     <t>Ressource</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>Mulden-Rigolen-Element</t>
+  </si>
+  <si>
+    <t>MAP-Fällung</t>
+  </si>
+  <si>
+    <t>Strippung und saure Wäsche</t>
   </si>
 </sst>
 </file>
@@ -313,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,18 +546,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" customWidth="1"/>
-    <col min="2" max="2" width="6.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -562,7 +568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -573,7 +579,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -584,7 +590,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -595,7 +601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -606,7 +612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -617,7 +623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -628,7 +634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -639,7 +645,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -650,7 +656,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
@@ -661,7 +667,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
@@ -672,7 +678,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -683,7 +689,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -694,7 +700,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -705,7 +711,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>3</v>
       </c>
@@ -716,7 +722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -727,7 +733,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>3</v>
       </c>
@@ -738,7 +744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -749,7 +755,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -760,7 +766,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -771,7 +777,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>5</v>
       </c>
@@ -782,7 +788,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>5</v>
       </c>
@@ -793,7 +799,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
@@ -804,7 +810,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -815,7 +821,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
@@ -826,7 +832,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>5</v>
       </c>
@@ -837,7 +843,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>5</v>
       </c>
@@ -848,7 +854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>5</v>
       </c>
@@ -859,25 +865,29 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="6">
         <v>9</v>
       </c>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="6">
         <v>10</v>
       </c>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>6</v>
       </c>
@@ -888,7 +898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>6</v>
       </c>
@@ -899,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>6</v>
       </c>
@@ -910,7 +920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>6</v>
       </c>
@@ -921,7 +931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>6</v>
       </c>
@@ -932,7 +942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>6</v>
       </c>
@@ -941,7 +951,7 @@
       </c>
       <c r="C36" s="8"/>
     </row>
-    <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>6</v>
       </c>
@@ -950,7 +960,7 @@
       </c>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>6</v>
       </c>
@@ -959,7 +969,7 @@
       </c>
       <c r="C38" s="8"/>
     </row>
-    <row r="39" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>6</v>
       </c>
@@ -968,7 +978,7 @@
       </c>
       <c r="C39" s="8"/>
     </row>
-    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>6</v>
       </c>
@@ -977,7 +987,7 @@
       </c>
       <c r="C40" s="8"/>
     </row>
-    <row r="41" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>12</v>
       </c>
@@ -988,7 +998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>12</v>
       </c>
@@ -999,7 +1009,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +1042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>12</v>
       </c>
@@ -1043,7 +1053,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1064,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>12</v>
       </c>
@@ -1065,7 +1075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>12</v>
       </c>
@@ -1076,7 +1086,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>12</v>
       </c>
@@ -1087,7 +1097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1108,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>12</v>
       </c>
@@ -1109,7 +1119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>12</v>
       </c>
@@ -1120,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>12</v>
       </c>
@@ -1142,7 +1152,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>12</v>
       </c>
@@ -1153,7 +1163,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>12</v>
       </c>
@@ -1164,7 +1174,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>12</v>
       </c>
@@ -1175,7 +1185,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>12</v>
       </c>
@@ -1186,7 +1196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1207,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>12</v>
       </c>
@@ -1208,7 +1218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>33</v>
       </c>
@@ -1217,7 +1227,7 @@
       </c>
       <c r="C62" s="13"/>
     </row>
-    <row r="63" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>33</v>
       </c>
@@ -1226,7 +1236,7 @@
       </c>
       <c r="C63" s="13"/>
     </row>
-    <row r="64" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>33</v>
       </c>
@@ -1235,7 +1245,7 @@
       </c>
       <c r="C64" s="13"/>
     </row>
-    <row r="65" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>33</v>
       </c>
@@ -1244,7 +1254,7 @@
       </c>
       <c r="C65" s="13"/>
     </row>
-    <row r="66" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>33</v>
       </c>
@@ -1253,7 +1263,7 @@
       </c>
       <c r="C66" s="13"/>
     </row>
-    <row r="67" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
         <v>33</v>
       </c>
@@ -1262,7 +1272,7 @@
       </c>
       <c r="C67" s="13"/>
     </row>
-    <row r="68" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
         <v>33</v>
       </c>
@@ -1271,7 +1281,7 @@
       </c>
       <c r="C68" s="13"/>
     </row>
-    <row r="69" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>33</v>
       </c>
@@ -1280,7 +1290,7 @@
       </c>
       <c r="C69" s="13"/>
     </row>
-    <row r="70" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
         <v>33</v>
       </c>
@@ -1289,7 +1299,7 @@
       </c>
       <c r="C70" s="13"/>
     </row>
-    <row r="71" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
         <v>33</v>
       </c>
@@ -1300,20 +1310,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003B6FAB07E96C754F884853C4F8523109" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="9dd0d1bcd91ccd6d35e6958805f3c92e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56655cf2-e854-4198-842a-b843eaa2cdb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c536939b36f29a2c70486bfcecf9ea4d" ns2:_="">
     <xsd:import namespace="56655cf2-e854-4198-842a-b843eaa2cdb6"/>
@@ -1445,6 +1446,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1452,14 +1462,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4EC041-2EC1-4BDF-84CB-6B1F4BDF1F23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92346914-4116-4F18-A3A7-DDCA20D55153}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1477,6 +1479,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4EC041-2EC1-4BDF-84CB-6B1F4BDF1F23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3A898C-DE27-4B67-B875-6A80314BF0C3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
entry for Gebäudepass_Altbau removed because only necessary in mysql database
</commit_message>
<xml_diff>
--- a/Massnahmenliste.xlsx
+++ b/Massnahmenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\R\R2Q_App\R2Q_App_VCurrent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197F4C31-4441-42CF-AAF7-847B452679D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039048F4-7A27-4506-A0C2-4D88CCDB358D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17910" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="62">
   <si>
     <t>Ressource</t>
   </si>
@@ -216,9 +216,6 @@
   </si>
   <si>
     <t>Strippung und saure Wäsche</t>
-  </si>
-  <si>
-    <t>Gebäudepass-Altbau</t>
   </si>
 </sst>
 </file>
@@ -558,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,9 +958,7 @@
       <c r="B36" s="8">
         <v>6</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
@@ -1329,21 +1324,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101003B6FAB07E96C754F884853C4F8523109" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="9dd0d1bcd91ccd6d35e6958805f3c92e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="56655cf2-e854-4198-842a-b843eaa2cdb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c536939b36f29a2c70486bfcecf9ea4d" ns2:_="">
     <xsd:import namespace="56655cf2-e854-4198-842a-b843eaa2cdb6"/>
@@ -1475,24 +1455,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3A898C-DE27-4B67-B875-6A80314BF0C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4EC041-2EC1-4BDF-84CB-6B1F4BDF1F23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92346914-4116-4F18-A3A7-DDCA20D55153}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1508,4 +1486,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4EC041-2EC1-4BDF-84CB-6B1F4BDF1F23}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA3A898C-DE27-4B67-B875-6A80314BF0C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>